<commit_message>
add xlsx. update Sheet4ver2.kt
</commit_message>
<xml_diff>
--- a/HMI_Screen_NHANDT53 - Copy.xlsx
+++ b/HMI_Screen_NHANDT53 - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daotr\Documents\AndroidStudioProjects\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3158CE-C64A-48C8-9A39-E490116B6CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF2F13E-FEA0-4183-A65E-D97655621AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2277" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2291" uniqueCount="360">
   <si>
     <t>Normal</t>
   </si>
@@ -1804,10 +1804,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51041F2-C0F6-4482-A04A-1F132E23BDEF}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:H88"/>
+  <dimension ref="B1:H90"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3825,6 +3825,52 @@
         <v>232</v>
       </c>
     </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B89" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B90" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3836,8 +3882,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="E2:O36"/>
   <sheetViews>
-    <sheetView topLeftCell="O9" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView topLeftCell="I7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7761,8 +7807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D486DB9-5481-4905-9349-77D8B5161CFF}">
   <dimension ref="D3:J111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="F85" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94:J95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>